<commit_message>
QA Compiler: Fix Excel safety, UNHIDE bug, and DAILY delta calculation
- Add sanitize_for_excel() to prevent formula injection (=, +, @)
- Fix UNHIDE bug: reset sheets/columns to visible before re-processing
- Fix DAILY tab: show daily delta (today - yesterday) not cumulative
- Apply fixes to both data display and chart data

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -1620,20 +1620,24 @@
           <t>--</t>
         </is>
       </c>
-      <c r="J7" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="K7" s="8" t="n">
-        <v>2</v>
+      <c r="J7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="L7" s="8" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="M7" s="8" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>--</t>
         </is>
       </c>
       <c r="N7" s="8" t="inlineStr">
@@ -1651,8 +1655,10 @@
           <t>--</t>
         </is>
       </c>
-      <c r="Q7" s="8" t="n">
-        <v>2</v>
+      <c r="Q7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -1694,14 +1700,14 @@
         </is>
       </c>
       <c r="J8" s="10" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K8" s="10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L8" s="10" t="inlineStr">
         <is>
-          <t>80.0%</t>
+          <t>40.0%</t>
         </is>
       </c>
       <c r="M8" s="10" t="inlineStr">
@@ -1719,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="Q8" s="10" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -1789,7 +1795,7 @@
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32">
@@ -1859,7 +1865,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QA Compiler: Fix Actual Issues % negative value bug
- Clamped actual_pct to 0-100% range using max(0, min(100, ...))
- Prevents -200% when nonissue count exceeds issues in daily delta
- Applied fix to all 7 occurrences (DAILY, TOTAL, charts)

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -1435,7 +1435,7 @@
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="F5" s="8" t="inlineStr">
@@ -1536,7 +1536,7 @@
       </c>
       <c r="I6" s="9" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J6" s="9" t="n">
@@ -1552,7 +1552,7 @@
       </c>
       <c r="M6" s="9" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N6" s="9" t="inlineStr">
@@ -1680,7 +1680,7 @@
       </c>
       <c r="E8" s="10" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="F8" s="10" t="n">
@@ -1696,7 +1696,7 @@
       </c>
       <c r="I8" s="10" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="J8" s="10" t="n">
@@ -1712,7 +1712,7 @@
       </c>
       <c r="M8" s="10" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="N8" s="10" t="n">
@@ -1986,7 +1986,7 @@
       </c>
       <c r="C3" s="8" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="D3" s="8" t="n">
@@ -2027,7 +2027,7 @@
       </c>
       <c r="C4" s="9" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="D4" s="9" t="n">
@@ -2068,7 +2068,7 @@
       </c>
       <c r="C5" s="8" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="D5" s="8" t="n">
@@ -2109,7 +2109,7 @@
       </c>
       <c r="C6" s="10" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="D6" s="10" t="n">
@@ -2157,7 +2157,7 @@
       </c>
       <c r="C9" s="10" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>100%</t>
         </is>
       </c>
       <c r="D9" s="10" t="n">

</xml_diff>

<commit_message>
QA Compiler: DAILY tab redesign - cleaner layout with thick borders
Changes:
- Remove Comp% and Actual Issues columns from DAILY (keep in TOTAL only)
- Add thick bold borders between users for clear visual separation
- Chart now uses main table directly (no separate data table)
- Simplified layout: only Done and Issues per user

Technical:
- tester_cols_per_user: 4 → 2
- Added thick_side border style for user separation
- Chart uses SeriesLabel for proper legend names
- Backwards compatible: _DAILY_DATA schema unchanged

Also updated:
- SYNC_THINKTANK.md with more planning details
- README.md with new DAILY tab layout documentation

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -93,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -115,11 +115,25 @@
         <color rgb="00000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="00000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -157,6 +171,26 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -262,9 +296,7 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <strRef>
-              <f>'DAILY'!B11</f>
-            </strRef>
+            <v>Alice</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -274,14 +306,9 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <cat>
-            <numRef>
-              <f>'DAILY'!$A$12:$A$14</f>
-            </numRef>
-          </cat>
           <val>
             <numRef>
-              <f>'DAILY'!$B$12:$B$14</f>
+              <f>'DAILY'!$B$5:$B$7</f>
             </numRef>
           </val>
         </ser>
@@ -289,9 +316,7 @@
           <idx val="1"/>
           <order val="1"/>
           <tx>
-            <strRef>
-              <f>'DAILY'!C11</f>
-            </strRef>
+            <v>Bob</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -301,14 +326,9 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <cat>
-            <numRef>
-              <f>'DAILY'!$A$12:$A$14</f>
-            </numRef>
-          </cat>
           <val>
             <numRef>
-              <f>'DAILY'!$C$12:$C$14</f>
+              <f>'DAILY'!$D$5:$D$7</f>
             </numRef>
           </val>
         </ser>
@@ -316,9 +336,7 @@
           <idx val="2"/>
           <order val="2"/>
           <tx>
-            <strRef>
-              <f>'DAILY'!D11</f>
-            </strRef>
+            <v>John</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -328,14 +346,9 @@
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <cat>
-            <numRef>
-              <f>'DAILY'!$A$12:$A$14</f>
-            </numRef>
-          </cat>
           <val>
             <numRef>
-              <f>'DAILY'!$D$12:$D$14</f>
+              <f>'DAILY'!$F$5:$F$7</f>
             </numRef>
           </val>
         </ser>
@@ -407,177 +420,6 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Daily Progress: Actual Issues % by Tester</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'DAILY'!B32</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'DAILY'!$A$33:$A$35</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'DAILY'!$B$33:$B$35</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>'DAILY'!C32</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="ED7D31"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'DAILY'!$A$33:$A$35</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'DAILY'!$C$33:$C$35</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>'DAILY'!D32</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="70AD47"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <cat>
-            <numRef>
-              <f>'DAILY'!$A$33:$A$35</f>
-            </numRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>'DAILY'!$D$33:$D$35</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Date</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <tickLblPos val="low"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Actual Issues %</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="b"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <style val="10"/>
   <chart>
@@ -721,7 +563,7 @@
 </chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <style val="10"/>
   <chart>
@@ -871,7 +713,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>16</row>
+      <row>9</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="3600000"/>
@@ -884,28 +726,6 @@
       <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>37</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="3600000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="2" name="Chart 2"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1252,7 +1072,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q35"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1263,20 +1083,14 @@
     <col width="8" customWidth="1" min="1" max="1"/>
     <col width="6" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="8" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="6" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="8" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="6" customWidth="1" min="10" max="10"/>
-    <col width="8" customWidth="1" min="11" max="11"/>
-    <col width="8" customWidth="1" min="12" max="12"/>
-    <col width="15" customWidth="1" min="13" max="13"/>
-    <col width="7" customWidth="1" min="14" max="14"/>
-    <col width="10" customWidth="1" min="15" max="15"/>
-    <col width="10" customWidth="1" min="16" max="16"/>
-    <col width="9" customWidth="1" min="17" max="17"/>
+    <col width="7" customWidth="1" min="8" max="8"/>
+    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="10" customWidth="1" min="10" max="10"/>
+    <col width="9" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1292,7 +1106,7 @@
           <t>Tester Stats</t>
         </is>
       </c>
-      <c r="N2" s="3" t="inlineStr">
+      <c r="H2" s="3" t="inlineStr">
         <is>
           <t>Manager Stats</t>
         </is>
@@ -1300,46 +1114,40 @@
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
-      <c r="B3" s="2" t="inlineStr">
+      <c r="B3" s="15" t="inlineStr">
         <is>
           <t>Alice</t>
         </is>
       </c>
-      <c r="C3" s="4" t="n"/>
-      <c r="D3" s="4" t="n"/>
-      <c r="E3" s="4" t="n"/>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="C3" s="16" t="n"/>
+      <c r="D3" s="15" t="inlineStr">
         <is>
           <t>Bob</t>
         </is>
       </c>
-      <c r="G3" s="4" t="n"/>
-      <c r="H3" s="4" t="n"/>
-      <c r="I3" s="4" t="n"/>
-      <c r="J3" s="2" t="inlineStr">
+      <c r="E3" s="16" t="n"/>
+      <c r="F3" s="15" t="inlineStr">
         <is>
           <t>John</t>
         </is>
       </c>
-      <c r="K3" s="4" t="n"/>
-      <c r="L3" s="4" t="n"/>
-      <c r="M3" s="4" t="n"/>
-      <c r="N3" s="5" t="inlineStr">
+      <c r="G3" s="16" t="n"/>
+      <c r="H3" s="17" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="O3" s="5" t="inlineStr">
+      <c r="I3" s="5" t="inlineStr">
         <is>
           <t>Reported</t>
         </is>
       </c>
-      <c r="P3" s="5" t="inlineStr">
+      <c r="J3" s="5" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
-      <c r="Q3" s="5" t="inlineStr">
+      <c r="K3" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1351,7 +1159,7 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="18" t="inlineStr">
         <is>
           <t>Done</t>
         </is>
@@ -1361,17 +1169,17 @@
           <t>Issues</t>
         </is>
       </c>
-      <c r="D4" s="6" t="inlineStr">
-        <is>
-          <t>Comp %</t>
+      <c r="D4" s="18" t="inlineStr">
+        <is>
+          <t>Done</t>
         </is>
       </c>
       <c r="E4" s="6" t="inlineStr">
         <is>
-          <t>Actual Issues</t>
-        </is>
-      </c>
-      <c r="F4" s="6" t="inlineStr">
+          <t>Issues</t>
+        </is>
+      </c>
+      <c r="F4" s="18" t="inlineStr">
         <is>
           <t>Done</t>
         </is>
@@ -1381,40 +1189,10 @@
           <t>Issues</t>
         </is>
       </c>
-      <c r="H4" s="6" t="inlineStr">
-        <is>
-          <t>Comp %</t>
-        </is>
-      </c>
-      <c r="I4" s="6" t="inlineStr">
-        <is>
-          <t>Actual Issues</t>
-        </is>
-      </c>
-      <c r="J4" s="6" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-      <c r="K4" s="6" t="inlineStr">
-        <is>
-          <t>Issues</t>
-        </is>
-      </c>
-      <c r="L4" s="6" t="inlineStr">
-        <is>
-          <t>Comp %</t>
-        </is>
-      </c>
-      <c r="M4" s="6" t="inlineStr">
-        <is>
-          <t>Actual Issues</t>
-        </is>
-      </c>
-      <c r="N4" s="7" t="n"/>
-      <c r="O4" s="7" t="n"/>
-      <c r="P4" s="7" t="n"/>
-      <c r="Q4" s="7" t="n"/>
+      <c r="H4" s="19" t="n"/>
+      <c r="I4" s="7" t="n"/>
+      <c r="J4" s="7" t="n"/>
+      <c r="K4" s="7" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
@@ -1422,23 +1200,23 @@
           <t>01/04</t>
         </is>
       </c>
-      <c r="B5" s="8" t="n">
+      <c r="B5" s="20" t="n">
         <v>5</v>
       </c>
       <c r="C5" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="D5" s="8" t="inlineStr">
-        <is>
-          <t>100.0%</t>
+      <c r="D5" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="F5" s="8" t="inlineStr">
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F5" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1448,7 +1226,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="H5" s="8" t="inlineStr">
+      <c r="H5" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1463,37 +1241,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="K5" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="L5" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="M5" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="N5" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="O5" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="P5" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="Q5" s="8" t="n">
+      <c r="K5" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1503,7 +1251,7 @@
           <t>01/05</t>
         </is>
       </c>
-      <c r="B6" s="9" t="inlineStr">
+      <c r="B6" s="21" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1513,64 +1261,34 @@
           <t>--</t>
         </is>
       </c>
-      <c r="D6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="E6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="F6" s="9" t="n">
+      <c r="D6" s="21" t="n">
         <v>3</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="F6" s="21" t="n">
+        <v>4</v>
       </c>
       <c r="G6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="9" t="inlineStr">
-        <is>
-          <t>100.0%</t>
+      <c r="H6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
         </is>
       </c>
       <c r="I6" s="9" t="inlineStr">
         <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="J6" s="9" t="n">
-        <v>4</v>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="J6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="K6" s="9" t="n">
-        <v>2</v>
-      </c>
-      <c r="L6" s="9" t="inlineStr">
-        <is>
-          <t>80.0%</t>
-        </is>
-      </c>
-      <c r="M6" s="9" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="N6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="O6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="P6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="Q6" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1580,7 +1298,7 @@
           <t>01/06</t>
         </is>
       </c>
-      <c r="B7" s="8" t="inlineStr">
+      <c r="B7" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1590,7 +1308,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="D7" s="8" t="inlineStr">
+      <c r="D7" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1600,7 +1318,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="F7" s="8" t="inlineStr">
+      <c r="F7" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1610,7 +1328,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="H7" s="8" t="inlineStr">
+      <c r="H7" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1626,36 +1344,6 @@
         </is>
       </c>
       <c r="K7" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="L7" s="8" t="inlineStr">
-        <is>
-          <t>0.0%</t>
-        </is>
-      </c>
-      <c r="M7" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="N7" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="O7" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="P7" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="Q7" s="8" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1667,215 +1355,45 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B8" s="10" t="n">
+      <c r="B8" s="22" t="n">
         <v>5</v>
       </c>
       <c r="C8" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="10" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-      <c r="E8" s="10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="F8" s="10" t="n">
+      <c r="D8" s="22" t="n">
         <v>3</v>
+      </c>
+      <c r="E8" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" s="22" t="n">
+        <v>4</v>
       </c>
       <c r="G8" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="10" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-      <c r="I8" s="10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="H8" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10" t="n">
+        <v>0</v>
       </c>
       <c r="J8" s="10" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K8" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="L8" s="10" t="inlineStr">
-        <is>
-          <t>40.0%</t>
-        </is>
-      </c>
-      <c r="M8" s="10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="N8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="O8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="P8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="10" t="n">
         <v>5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B11" s="11" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="C11" s="11" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="D11" s="11" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>01/04</t>
-        </is>
-      </c>
-      <c r="B12" t="n">
-        <v>5</v>
-      </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>01/05</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>0</v>
-      </c>
-      <c r="C13" t="n">
-        <v>3</v>
-      </c>
-      <c r="D13" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>01/06</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>0</v>
-      </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="B32" s="11" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="C32" s="11" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="D32" s="11" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>01/04</t>
-        </is>
-      </c>
-      <c r="B33" t="n">
-        <v>100</v>
-      </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>01/05</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>0</v>
-      </c>
-      <c r="C34" t="n">
-        <v>100</v>
-      </c>
-      <c r="D34" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>01/06</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>0</v>
-      </c>
-      <c r="C35" t="n">
-        <v>0</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="B2:M2"/>
-    <mergeCell ref="F3:I3"/>
-    <mergeCell ref="J3:M3"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
QA Compiler: Fix corrupted Excel filter error with safe_load_workbook
Problem:
- openpyxl crashes on Excel files with corrupted auto-filter values
- Error: "Value must be either numerical or a string containing a wildcard"
- Prevents processing valid QA work in affected files

Solution:
- Added safe_load_workbook() wrapper function
- Catches filter corruption errors
- Attempts recovery with data_only=True
- Provides clear error message with fix instructions:
  "Open in Excel → Data → Clear filters → Save → Retry"

Also includes DAILY tab redesign from previous commit.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -93,7 +93,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -128,6 +128,39 @@
       <bottom style="thin">
         <color rgb="00000000"/>
       </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="00000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="00000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="00000000"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">

</xml_diff>

<commit_message>
QA Compiler: TOTAL tab improvements - cleaner header and charts
Changes:
1. Header: "Comp %" → "Completion" (clearer label)
2. Charts now use MAIN TABLE directly (no separate data tables)
   - References user data rows from main table columns
   - Column 4 (Total/Done) for Done chart
   - Column 3 (Actual Issues) for Issues chart
   - Cleaner, consistent with DAILY tab approach

Technical:
- Added user_row_tracker to build_section() to track data row numbers
- Charts reference tracked rows directly from main table
- Each user becomes a series with their name in legend
- No more separate "Tester | Done" data tables below main content

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -479,56 +479,59 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <strRef>
-              <f>'TOTAL'!B12</f>
-            </strRef>
+            <v>Alice</v>
           </tx>
           <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
             <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <dPt>
-            <idx val="0"/>
-            <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <dPt>
-            <idx val="1"/>
-            <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:srgbClr val="ED7D31"/>
-              </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <dPt>
-            <idx val="2"/>
-            <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:srgbClr val="70AD47"/>
-              </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <cat>
-            <numRef>
-              <f>'TOTAL'!$A$13:$A$15</f>
-            </numRef>
-          </cat>
           <val>
             <numRef>
-              <f>'TOTAL'!$B$13:$B$15</f>
+              <f>'TOTAL'!$D$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Bob</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>John</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="70AD47"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$5</f>
             </numRef>
           </val>
         </ser>
@@ -541,25 +544,10 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
+        <delete val="1"/>
         <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Tester</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="low"/>
         <crossAx val="100"/>
         <lblOffset val="100"/>
       </catAx>
@@ -590,6 +578,9 @@
         <crossAx val="10"/>
       </valAx>
     </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
@@ -623,56 +614,59 @@
           <idx val="0"/>
           <order val="0"/>
           <tx>
-            <strRef>
-              <f>'TOTAL'!B33</f>
-            </strRef>
+            <v>Alice</v>
           </tx>
           <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
             <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
-          <dPt>
-            <idx val="0"/>
-            <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:srgbClr val="4472C4"/>
-              </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <dPt>
-            <idx val="1"/>
-            <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:srgbClr val="ED7D31"/>
-              </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <dPt>
-            <idx val="2"/>
-            <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:srgbClr val="70AD47"/>
-              </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </dPt>
-          <cat>
-            <numRef>
-              <f>'TOTAL'!$A$34:$A$36</f>
-            </numRef>
-          </cat>
           <val>
             <numRef>
-              <f>'TOTAL'!$B$34:$B$36</f>
+              <f>'TOTAL'!$C$3</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <v>Bob</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="ED7D31"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$4</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <v>John</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="70AD47"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$5</f>
             </numRef>
           </val>
         </ser>
@@ -685,25 +679,10 @@
         <scaling>
           <orientation val="minMax"/>
         </scaling>
+        <delete val="1"/>
         <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Tester</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
-        <tickLblPos val="low"/>
         <crossAx val="100"/>
         <lblOffset val="100"/>
       </catAx>
@@ -734,6 +713,9 @@
         <crossAx val="10"/>
       </valAx>
     </plotArea>
+    <legend>
+      <legendPos val="b"/>
+    </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
   </chart>
@@ -773,7 +755,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>17</row>
+      <row>11</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="3600000"/>
@@ -795,7 +777,7 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>38</row>
+      <row>26</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="5400000" cy="3600000"/>
@@ -1439,7 +1421,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K36"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1448,7 +1430,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
     <col width="7" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
@@ -1475,7 +1457,7 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>Comp %</t>
+          <t>Completion</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
@@ -1734,90 +1716,6 @@
       </c>
       <c r="K9" s="10" t="n">
         <v>7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Tester</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Done</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="B13" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="B14" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>Tester</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>Actual Issues %</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>Alice</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Bob</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>John</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QA Compiler: Cleanup and reorganize project
- Remove fake test files (Alice_Quest, Bob_Knowledge, old LQA_Quest.xlsx)
- Move datasheet scripts from "DATASHEET SCRIPTS 0108" to datasheet_generators/
- Add CODE_REVIEW_REPORT and STRINGID_MATCHING_PLAN docs
- Keep only real QA files: Quest, Knowledge, Item, Region, Character

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -18,7 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0&quot;%&quot;"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <name val="Calibri"/>
@@ -166,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -224,6 +226,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -341,7 +352,7 @@
           </spPr>
           <val>
             <numRef>
-              <f>'DAILY'!$B$5:$B$7</f>
+              <f>'DAILY'!$B$5:$B$8</f>
             </numRef>
           </val>
         </ser>
@@ -361,7 +372,7 @@
           </spPr>
           <val>
             <numRef>
-              <f>'DAILY'!$D$5:$D$7</f>
+              <f>'DAILY'!$D$5:$D$8</f>
             </numRef>
           </val>
         </ser>
@@ -369,7 +380,7 @@
           <idx val="2"/>
           <order val="2"/>
           <tx>
-            <v>John</v>
+            <v>Doni</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -381,7 +392,107 @@
           </spPr>
           <val>
             <numRef>
-              <f>'DAILY'!$F$5:$F$7</f>
+              <f>'DAILY'!$F$5:$F$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>John</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'DAILY'!$H$5:$H$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Jojo</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="5B9BD5"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'DAILY'!$J$5:$J$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Lisa</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'DAILY'!$L$5:$L$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Mike</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'DAILY'!$N$5:$N$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Paul</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'DAILY'!$P$5:$P$8</f>
             </numRef>
           </val>
         </ser>
@@ -519,7 +630,7 @@
           <idx val="2"/>
           <order val="2"/>
           <tx>
-            <v>John</v>
+            <v>Doni</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -532,6 +643,106 @@
           <val>
             <numRef>
               <f>'TOTAL'!$D$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>John</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Jojo</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="5B9BD5"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Lisa</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Mike</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Paul</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$10</f>
             </numRef>
           </val>
         </ser>
@@ -654,7 +865,7 @@
           <idx val="2"/>
           <order val="2"/>
           <tx>
-            <v>John</v>
+            <v>Doni</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -667,6 +878,106 @@
           <val>
             <numRef>
               <f>'TOTAL'!$C$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <v>John</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$6</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <v>Jojo</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="5B9BD5"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <v>Lisa</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="7030A0"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="6"/>
+          <order val="6"/>
+          <tx>
+            <v>Mike</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="C00000"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$9</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="7"/>
+          <order val="7"/>
+          <tx>
+            <v>Paul</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="00B0F0"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$10</f>
             </numRef>
           </val>
         </ser>
@@ -755,10 +1066,10 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>11</row>
+      <row>16</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5400000" cy="3600000"/>
+    <ext cx="7920000" cy="3600000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -777,10 +1088,10 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>26</row>
+      <row>31</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="5400000" cy="3600000"/>
+    <ext cx="7920000" cy="3600000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="2" name="Chart 2"/>
@@ -1087,7 +1398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1102,10 +1413,21 @@
     <col width="8" customWidth="1" min="5" max="5"/>
     <col width="6" customWidth="1" min="6" max="6"/>
     <col width="8" customWidth="1" min="7" max="7"/>
-    <col width="7" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="9" customWidth="1" min="11" max="11"/>
+    <col width="6" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="9" max="9"/>
+    <col width="6" customWidth="1" min="10" max="10"/>
+    <col width="8" customWidth="1" min="11" max="11"/>
+    <col width="6" customWidth="1" min="12" max="12"/>
+    <col width="8" customWidth="1" min="13" max="13"/>
+    <col width="6" customWidth="1" min="14" max="14"/>
+    <col width="8" customWidth="1" min="15" max="15"/>
+    <col width="6" customWidth="1" min="16" max="16"/>
+    <col width="8" customWidth="1" min="17" max="17"/>
+    <col width="7" customWidth="1" min="18" max="18"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="10" customWidth="1" min="21" max="21"/>
+    <col width="9" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1121,7 +1443,7 @@
           <t>Tester Stats</t>
         </is>
       </c>
-      <c r="H2" s="3" t="inlineStr">
+      <c r="R2" s="3" t="inlineStr">
         <is>
           <t>Manager Stats</t>
         </is>
@@ -1143,26 +1465,61 @@
       <c r="E3" s="16" t="n"/>
       <c r="F3" s="15" t="inlineStr">
         <is>
+          <t>Doni</t>
+        </is>
+      </c>
+      <c r="G3" s="16" t="n"/>
+      <c r="H3" s="15" t="inlineStr">
+        <is>
           <t>John</t>
         </is>
       </c>
-      <c r="G3" s="16" t="n"/>
-      <c r="H3" s="17" t="inlineStr">
+      <c r="I3" s="16" t="n"/>
+      <c r="J3" s="15" t="inlineStr">
+        <is>
+          <t>Jojo</t>
+        </is>
+      </c>
+      <c r="K3" s="16" t="n"/>
+      <c r="L3" s="15" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="M3" s="16" t="n"/>
+      <c r="N3" s="15" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="O3" s="16" t="n"/>
+      <c r="P3" s="15" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="Q3" s="16" t="n"/>
+      <c r="R3" s="17" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="I3" s="5" t="inlineStr">
+      <c r="S3" s="5" t="inlineStr">
         <is>
           <t>Reported</t>
         </is>
       </c>
-      <c r="J3" s="5" t="inlineStr">
+      <c r="T3" s="5" t="inlineStr">
+        <is>
+          <t>NonIssue</t>
+        </is>
+      </c>
+      <c r="U3" s="5" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
-      <c r="K3" s="5" t="inlineStr">
+      <c r="V3" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1204,10 +1561,61 @@
           <t>Issues</t>
         </is>
       </c>
-      <c r="H4" s="19" t="n"/>
-      <c r="I4" s="7" t="n"/>
-      <c r="J4" s="7" t="n"/>
-      <c r="K4" s="7" t="n"/>
+      <c r="H4" s="18" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="I4" s="6" t="inlineStr">
+        <is>
+          <t>Issues</t>
+        </is>
+      </c>
+      <c r="J4" s="18" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="K4" s="6" t="inlineStr">
+        <is>
+          <t>Issues</t>
+        </is>
+      </c>
+      <c r="L4" s="18" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="M4" s="6" t="inlineStr">
+        <is>
+          <t>Issues</t>
+        </is>
+      </c>
+      <c r="N4" s="18" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="O4" s="6" t="inlineStr">
+        <is>
+          <t>Issues</t>
+        </is>
+      </c>
+      <c r="P4" s="18" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="Q4" s="6" t="inlineStr">
+        <is>
+          <t>Issues</t>
+        </is>
+      </c>
+      <c r="R4" s="19" t="n"/>
+      <c r="S4" s="7" t="n"/>
+      <c r="T4" s="7" t="n"/>
+      <c r="U4" s="7" t="n"/>
+      <c r="V4" s="7" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
@@ -1251,12 +1659,67 @@
           <t>--</t>
         </is>
       </c>
-      <c r="J5" s="8" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="K5" s="8" t="n">
+      <c r="J5" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L5" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N5" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="P5" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Q5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R5" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="S5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="U5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V5" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1282,28 +1745,83 @@
       <c r="E6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="21" t="n">
+      <c r="F6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H6" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="I6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="I6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="J6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="K6" s="9" t="n">
+      <c r="J6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="K6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="L6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="P6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Q6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="S6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="U6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V6" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1353,7 +1871,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="J7" s="8" t="inlineStr">
+      <c r="J7" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1363,52 +1881,169 @@
           <t>--</t>
         </is>
       </c>
+      <c r="L7" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N7" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="P7" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="Q7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="R7" s="20" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="S7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="U7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="10" t="inlineStr">
-        <is>
-          <t>TOTAL</t>
-        </is>
-      </c>
-      <c r="B8" s="22" t="n">
-        <v>5</v>
-      </c>
-      <c r="C8" s="10" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="22" t="n">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>01/09</t>
+        </is>
+      </c>
+      <c r="B8" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="C8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="D8" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="E8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="F8" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="G8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="H8" s="21" t="n">
+        <v>338</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="J8" s="21" t="n">
+        <v>30</v>
+      </c>
+      <c r="K8" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="E8" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="F8" s="22" t="n">
-        <v>4</v>
-      </c>
-      <c r="G8" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="10" t="n">
-        <v>5</v>
+      <c r="L8" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="M8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="N8" s="21" t="n">
+        <v>229</v>
+      </c>
+      <c r="O8" s="9" t="n">
+        <v>76</v>
+      </c>
+      <c r="P8" s="21" t="n">
+        <v>229</v>
+      </c>
+      <c r="Q8" s="9" t="n">
+        <v>55</v>
+      </c>
+      <c r="R8" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="S8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="T8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="U8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="V8" s="9" t="n">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="11">
     <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="N3:O3"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="H2:K2"/>
+    <mergeCell ref="A1:V1"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="B2:Q2"/>
     <mergeCell ref="D3:E3"/>
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -1421,7 +2056,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1512,15 +2147,11 @@
           <t>Alice</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-      <c r="C3" s="8" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="B3" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="C3" s="23" t="n">
+        <v>100</v>
       </c>
       <c r="D3" s="8" t="n">
         <v>5</v>
@@ -1553,15 +2184,11 @@
           <t>Bob</t>
         </is>
       </c>
-      <c r="B4" s="9" t="inlineStr">
-        <is>
-          <t>100.0%</t>
-        </is>
-      </c>
-      <c r="C4" s="9" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
+      <c r="B4" s="24" t="n">
+        <v>100</v>
+      </c>
+      <c r="C4" s="24" t="n">
+        <v>100</v>
       </c>
       <c r="D4" s="9" t="n">
         <v>3</v>
@@ -1591,137 +2218,310 @@
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
         <is>
+          <t>Doni</t>
+        </is>
+      </c>
+      <c r="B5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="9" t="inlineStr">
+        <is>
           <t>John</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
-        <is>
-          <t>80.0%</t>
-        </is>
-      </c>
-      <c r="C5" s="8" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="D5" s="8" t="n">
-        <v>8</v>
-      </c>
-      <c r="E5" s="8" t="n">
-        <v>4</v>
-      </c>
-      <c r="F5" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="B6" s="24" t="n">
+        <v>90.09999999999999</v>
+      </c>
+      <c r="C6" s="24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>346</v>
+      </c>
+      <c r="E6" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="9" t="n">
+        <v>319</v>
+      </c>
+      <c r="G6" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="H6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>Jojo</t>
+        </is>
+      </c>
+      <c r="B7" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" s="8" t="n">
+        <v>30</v>
+      </c>
+      <c r="E7" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8" t="n">
+        <v>27</v>
+      </c>
+      <c r="G7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="9" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="B8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="8" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="B9" s="23" t="n">
+        <v>89.09999999999999</v>
+      </c>
+      <c r="C9" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" s="8" t="n">
+        <v>229</v>
+      </c>
+      <c r="E9" s="8" t="n">
+        <v>76</v>
+      </c>
+      <c r="F9" s="8" t="n">
+        <v>153</v>
+      </c>
+      <c r="G9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="8" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="9" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B10" s="24" t="n">
+        <v>89.09999999999999</v>
+      </c>
+      <c r="C10" s="24" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>229</v>
+      </c>
+      <c r="E10" s="9" t="n">
+        <v>55</v>
+      </c>
+      <c r="F10" s="9" t="n">
+        <v>174</v>
+      </c>
+      <c r="G10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="9" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="10" t="inlineStr">
         <is>
           <t>SUBTOTAL</t>
         </is>
       </c>
-      <c r="B6" s="10" t="inlineStr">
-        <is>
-          <t>88.9%</t>
-        </is>
-      </c>
-      <c r="C6" s="10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="D6" s="10" t="n">
-        <v>16</v>
-      </c>
-      <c r="E6" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="F6" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="G6" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="10" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="14" t="inlineStr">
+      <c r="B11" s="25" t="n">
+        <v>86.59999999999999</v>
+      </c>
+      <c r="C11" s="25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" s="10" t="n">
+        <v>842</v>
+      </c>
+      <c r="E11" s="10" t="n">
+        <v>147</v>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>678</v>
+      </c>
+      <c r="G11" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="H11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="10" t="n">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="14" t="inlineStr">
         <is>
           <t>GRAND TOTAL (ALL LANGUAGES)</t>
         </is>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="10" t="inlineStr">
+    <row r="14">
+      <c r="A14" s="10" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B9" s="10" t="inlineStr">
-        <is>
-          <t>88.9%</t>
-        </is>
-      </c>
-      <c r="C9" s="10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="D9" s="10" t="n">
-        <v>16</v>
-      </c>
-      <c r="E9" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="F9" s="10" t="n">
-        <v>7</v>
-      </c>
-      <c r="G9" s="10" t="n">
-        <v>2</v>
-      </c>
-      <c r="H9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="10" t="n">
-        <v>7</v>
+      <c r="B14" s="25" t="n">
+        <v>86.59999999999999</v>
+      </c>
+      <c r="C14" s="25" t="n">
+        <v>100</v>
+      </c>
+      <c r="D14" s="10" t="n">
+        <v>842</v>
+      </c>
+      <c r="E14" s="10" t="n">
+        <v>147</v>
+      </c>
+      <c r="F14" s="10" t="n">
+        <v>678</v>
+      </c>
+      <c r="G14" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="H14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K14" s="10" t="n">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A13:K13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -1734,7 +2534,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1980,6 +2780,270 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Doni</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Knowledge</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>379</v>
+      </c>
+      <c r="E7" t="n">
+        <v>342</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8</v>
+      </c>
+      <c r="G7" t="n">
+        <v>318</v>
+      </c>
+      <c r="H7" t="n">
+        <v>16</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>257</v>
+      </c>
+      <c r="E8" t="n">
+        <v>229</v>
+      </c>
+      <c r="F8" t="n">
+        <v>76</v>
+      </c>
+      <c r="G8" t="n">
+        <v>153</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>36</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>257</v>
+      </c>
+      <c r="E10" t="n">
+        <v>229</v>
+      </c>
+      <c r="F10" t="n">
+        <v>55</v>
+      </c>
+      <c r="G10" t="n">
+        <v>174</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Jojo</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Character</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>30</v>
+      </c>
+      <c r="E11" t="n">
+        <v>30</v>
+      </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
+      <c r="G11" t="n">
+        <v>27</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
QA Compiler: Add mock data to Quest files for testing
- Added 14 STATUS entries to John_Quest (ENG)
- Added 3 STATUS entries to Eric_Quest (FRE)
- Updated Master files with transfer results

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -400,7 +400,7 @@
           <idx val="3"/>
           <order val="3"/>
           <tx>
-            <v>John</v>
+            <v>Eric</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -420,7 +420,7 @@
           <idx val="4"/>
           <order val="4"/>
           <tx>
-            <v>Jojo</v>
+            <v>John</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -440,7 +440,7 @@
           <idx val="5"/>
           <order val="5"/>
           <tx>
-            <v>Lisa</v>
+            <v>Jojo</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -460,7 +460,7 @@
           <idx val="6"/>
           <order val="6"/>
           <tx>
-            <v>Mike</v>
+            <v>Lisa</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -480,7 +480,7 @@
           <idx val="7"/>
           <order val="7"/>
           <tx>
-            <v>Paul</v>
+            <v>Mike</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -493,6 +493,26 @@
           <val>
             <numRef>
               <f>'DAILY'!$P$5:$P$8</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Paul</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'DAILY'!$R$5:$R$8</f>
             </numRef>
           </val>
         </ser>
@@ -650,7 +670,7 @@
           <idx val="3"/>
           <order val="3"/>
           <tx>
-            <v>John</v>
+            <v>Eric</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -670,7 +690,7 @@
           <idx val="4"/>
           <order val="4"/>
           <tx>
-            <v>Jojo</v>
+            <v>John</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -690,7 +710,7 @@
           <idx val="5"/>
           <order val="5"/>
           <tx>
-            <v>Lisa</v>
+            <v>Jojo</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -710,7 +730,7 @@
           <idx val="6"/>
           <order val="6"/>
           <tx>
-            <v>Mike</v>
+            <v>Lisa</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -730,7 +750,7 @@
           <idx val="7"/>
           <order val="7"/>
           <tx>
-            <v>Paul</v>
+            <v>Mike</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -743,6 +763,26 @@
           <val>
             <numRef>
               <f>'TOTAL'!$D$10</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Paul</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$D$11</f>
             </numRef>
           </val>
         </ser>
@@ -885,7 +925,7 @@
           <idx val="3"/>
           <order val="3"/>
           <tx>
-            <v>John</v>
+            <v>Eric</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -905,7 +945,7 @@
           <idx val="4"/>
           <order val="4"/>
           <tx>
-            <v>Jojo</v>
+            <v>John</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -925,7 +965,7 @@
           <idx val="5"/>
           <order val="5"/>
           <tx>
-            <v>Lisa</v>
+            <v>Jojo</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -945,7 +985,7 @@
           <idx val="6"/>
           <order val="6"/>
           <tx>
-            <v>Mike</v>
+            <v>Lisa</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -965,7 +1005,7 @@
           <idx val="7"/>
           <order val="7"/>
           <tx>
-            <v>Paul</v>
+            <v>Mike</v>
           </tx>
           <spPr>
             <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -978,6 +1018,26 @@
           <val>
             <numRef>
               <f>'TOTAL'!$C$10</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="8"/>
+          <order val="8"/>
+          <tx>
+            <v>Paul</v>
+          </tx>
+          <spPr>
+            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:srgbClr val="4472C4"/>
+            </a:solidFill>
+            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'TOTAL'!$C$11</f>
             </numRef>
           </val>
         </ser>
@@ -1066,10 +1126,10 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>16</row>
+      <row>17</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7920000" cy="3600000"/>
+    <ext cx="8640000" cy="3600000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -1088,10 +1148,10 @@
     <from>
       <col>0</col>
       <colOff>0</colOff>
-      <row>31</row>
+      <row>32</row>
       <rowOff>0</rowOff>
     </from>
-    <ext cx="7920000" cy="3600000"/>
+    <ext cx="8640000" cy="3600000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="2" name="Chart 2"/>
@@ -1398,7 +1458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V8"/>
+  <dimension ref="A1:X8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1423,11 +1483,13 @@
     <col width="8" customWidth="1" min="15" max="15"/>
     <col width="6" customWidth="1" min="16" max="16"/>
     <col width="8" customWidth="1" min="17" max="17"/>
-    <col width="7" customWidth="1" min="18" max="18"/>
-    <col width="10" customWidth="1" min="19" max="19"/>
-    <col width="10" customWidth="1" min="20" max="20"/>
+    <col width="6" customWidth="1" min="18" max="18"/>
+    <col width="8" customWidth="1" min="19" max="19"/>
+    <col width="7" customWidth="1" min="20" max="20"/>
     <col width="10" customWidth="1" min="21" max="21"/>
-    <col width="9" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="22" max="22"/>
+    <col width="10" customWidth="1" min="23" max="23"/>
+    <col width="9" customWidth="1" min="24" max="24"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1443,7 +1505,7 @@
           <t>Tester Stats</t>
         </is>
       </c>
-      <c r="R2" s="3" t="inlineStr">
+      <c r="T2" s="3" t="inlineStr">
         <is>
           <t>Manager Stats</t>
         </is>
@@ -1471,55 +1533,61 @@
       <c r="G3" s="16" t="n"/>
       <c r="H3" s="15" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="I3" s="16" t="n"/>
       <c r="J3" s="15" t="inlineStr">
         <is>
-          <t>Jojo</t>
+          <t>John</t>
         </is>
       </c>
       <c r="K3" s="16" t="n"/>
       <c r="L3" s="15" t="inlineStr">
         <is>
-          <t>Lisa</t>
+          <t>Jojo</t>
         </is>
       </c>
       <c r="M3" s="16" t="n"/>
       <c r="N3" s="15" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="O3" s="16" t="n"/>
       <c r="P3" s="15" t="inlineStr">
         <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="Q3" s="16" t="n"/>
+      <c r="R3" s="15" t="inlineStr">
+        <is>
           <t>Paul</t>
         </is>
       </c>
-      <c r="Q3" s="16" t="n"/>
-      <c r="R3" s="17" t="inlineStr">
+      <c r="S3" s="16" t="n"/>
+      <c r="T3" s="17" t="inlineStr">
         <is>
           <t>Fixed</t>
         </is>
       </c>
-      <c r="S3" s="5" t="inlineStr">
+      <c r="U3" s="5" t="inlineStr">
         <is>
           <t>Reported</t>
         </is>
       </c>
-      <c r="T3" s="5" t="inlineStr">
+      <c r="V3" s="5" t="inlineStr">
         <is>
           <t>NonIssue</t>
         </is>
       </c>
-      <c r="U3" s="5" t="inlineStr">
+      <c r="W3" s="5" t="inlineStr">
         <is>
           <t>Checking</t>
         </is>
       </c>
-      <c r="V3" s="5" t="inlineStr">
+      <c r="X3" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1611,11 +1679,21 @@
           <t>Issues</t>
         </is>
       </c>
-      <c r="R4" s="19" t="n"/>
-      <c r="S4" s="7" t="n"/>
-      <c r="T4" s="7" t="n"/>
+      <c r="R4" s="18" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="S4" s="6" t="inlineStr">
+        <is>
+          <t>Issues</t>
+        </is>
+      </c>
+      <c r="T4" s="19" t="n"/>
       <c r="U4" s="7" t="n"/>
       <c r="V4" s="7" t="n"/>
+      <c r="W4" s="7" t="n"/>
+      <c r="X4" s="7" t="n"/>
     </row>
     <row r="5">
       <c r="A5" s="8" t="inlineStr">
@@ -1709,7 +1787,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="T5" s="8" t="inlineStr">
+      <c r="T5" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1719,7 +1797,17 @@
           <t>--</t>
         </is>
       </c>
-      <c r="V5" s="8" t="n">
+      <c r="V5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="W5" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X5" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1755,22 +1843,22 @@
           <t>--</t>
         </is>
       </c>
-      <c r="H6" s="21" t="n">
+      <c r="H6" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="J6" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="I6" s="9" t="n">
+      <c r="K6" s="9" t="n">
         <v>2</v>
       </c>
-      <c r="J6" s="21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="K6" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
       <c r="L6" s="21" t="inlineStr">
         <is>
           <t>--</t>
@@ -1811,7 +1899,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="T6" s="9" t="inlineStr">
+      <c r="T6" s="21" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1821,7 +1909,17 @@
           <t>--</t>
         </is>
       </c>
-      <c r="V6" s="9" t="n">
+      <c r="V6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="W6" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X6" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1921,7 +2019,7 @@
           <t>--</t>
         </is>
       </c>
-      <c r="T7" s="8" t="inlineStr">
+      <c r="T7" s="20" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1932,6 +2030,16 @@
         </is>
       </c>
       <c r="V7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="W7" s="8" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X7" s="8" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -1973,51 +2081,51 @@
           <t>--</t>
         </is>
       </c>
-      <c r="H8" s="21" t="n">
-        <v>338</v>
-      </c>
-      <c r="I8" s="9" t="n">
-        <v>6</v>
+      <c r="H8" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="I8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="J8" s="21" t="n">
-        <v>30</v>
+        <v>343</v>
       </c>
       <c r="K8" s="9" t="n">
         <v>3</v>
       </c>
-      <c r="L8" s="21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="M8" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="N8" s="21" t="n">
-        <v>229</v>
-      </c>
-      <c r="O8" s="9" t="n">
-        <v>76</v>
+      <c r="L8" s="21" t="n">
+        <v>32</v>
+      </c>
+      <c r="M8" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="N8" s="21" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="O8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
       </c>
       <c r="P8" s="21" t="n">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="Q8" s="9" t="n">
-        <v>55</v>
-      </c>
-      <c r="R8" s="21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="S8" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="T8" s="9" t="inlineStr">
+        <v>84</v>
+      </c>
+      <c r="R8" s="21" t="n">
+        <v>249</v>
+      </c>
+      <c r="S8" s="9" t="n">
+        <v>63</v>
+      </c>
+      <c r="T8" s="21" t="inlineStr">
         <is>
           <t>--</t>
         </is>
@@ -2027,21 +2135,32 @@
           <t>--</t>
         </is>
       </c>
-      <c r="V8" s="9" t="n">
-        <v>140</v>
+      <c r="V8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="W8" s="9" t="inlineStr">
+        <is>
+          <t>--</t>
+        </is>
+      </c>
+      <c r="X8" s="9" t="n">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="N3:O3"/>
+    <mergeCell ref="B2:S2"/>
+    <mergeCell ref="T2:X2"/>
     <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A1:V1"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="B2:Q2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="A1:X1"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="H3:I3"/>
   </mergeCells>
@@ -2056,7 +2175,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2255,26 +2374,26 @@
     <row r="6">
       <c r="A6" s="9" t="inlineStr">
         <is>
-          <t>John</t>
+          <t>Eric</t>
         </is>
       </c>
       <c r="B6" s="24" t="n">
-        <v>90.09999999999999</v>
+        <v>0</v>
       </c>
       <c r="C6" s="24" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D6" s="9" t="n">
-        <v>346</v>
+        <v>0</v>
       </c>
       <c r="E6" s="9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F6" s="9" t="n">
-        <v>319</v>
+        <v>0</v>
       </c>
       <c r="G6" s="9" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="H6" s="9" t="n">
         <v>0</v>
@@ -2286,32 +2405,32 @@
         <v>0</v>
       </c>
       <c r="K6" s="9" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="8" t="inlineStr">
         <is>
-          <t>Jojo</t>
+          <t>John</t>
         </is>
       </c>
       <c r="B7" s="23" t="n">
-        <v>100</v>
+        <v>88.7</v>
       </c>
       <c r="C7" s="23" t="n">
         <v>100</v>
       </c>
       <c r="D7" s="8" t="n">
-        <v>30</v>
+        <v>347</v>
       </c>
       <c r="E7" s="8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>27</v>
+        <v>323</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="H7" s="8" t="n">
         <v>0</v>
@@ -2323,29 +2442,29 @@
         <v>0</v>
       </c>
       <c r="K7" s="8" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="9" t="inlineStr">
         <is>
-          <t>Lisa</t>
+          <t>Jojo</t>
         </is>
       </c>
       <c r="B8" s="24" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C8" s="24" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>0</v>
+        <v>32</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="G8" s="9" t="n">
         <v>0</v>
@@ -2360,29 +2479,29 @@
         <v>0</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="8" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="B9" s="23" t="n">
-        <v>89.09999999999999</v>
+        <v>0</v>
       </c>
       <c r="C9" s="23" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>229</v>
+        <v>0</v>
       </c>
       <c r="E9" s="8" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>153</v>
+        <v>0</v>
       </c>
       <c r="G9" s="8" t="n">
         <v>0</v>
@@ -2397,29 +2516,29 @@
         <v>0</v>
       </c>
       <c r="K9" s="8" t="n">
-        <v>76</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="9" t="inlineStr">
         <is>
-          <t>Paul</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="B10" s="24" t="n">
-        <v>89.09999999999999</v>
+        <v>95</v>
       </c>
       <c r="C10" s="24" t="n">
         <v>100</v>
       </c>
       <c r="D10" s="9" t="n">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="E10" s="9" t="n">
-        <v>55</v>
+        <v>84</v>
       </c>
       <c r="F10" s="9" t="n">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>0</v>
@@ -2434,94 +2553,131 @@
         <v>0</v>
       </c>
       <c r="K10" s="9" t="n">
-        <v>55</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="10" t="inlineStr">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B11" s="23" t="n">
+        <v>95</v>
+      </c>
+      <c r="C11" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" s="8" t="n">
+        <v>249</v>
+      </c>
+      <c r="E11" s="8" t="n">
+        <v>63</v>
+      </c>
+      <c r="F11" s="8" t="n">
+        <v>186</v>
+      </c>
+      <c r="G11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="10" t="inlineStr">
         <is>
           <t>SUBTOTAL</t>
         </is>
       </c>
-      <c r="B11" s="25" t="n">
-        <v>86.59999999999999</v>
-      </c>
-      <c r="C11" s="25" t="n">
+      <c r="B12" s="25" t="n">
+        <v>89.09999999999999</v>
+      </c>
+      <c r="C12" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="D11" s="10" t="n">
-        <v>842</v>
-      </c>
-      <c r="E11" s="10" t="n">
-        <v>147</v>
-      </c>
-      <c r="F11" s="10" t="n">
-        <v>678</v>
-      </c>
-      <c r="G11" s="10" t="n">
-        <v>17</v>
-      </c>
-      <c r="H11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="10" t="n">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="14" t="inlineStr">
+      <c r="D12" s="10" t="n">
+        <v>885</v>
+      </c>
+      <c r="E12" s="10" t="n">
+        <v>159</v>
+      </c>
+      <c r="F12" s="10" t="n">
+        <v>707</v>
+      </c>
+      <c r="G12" s="10" t="n">
+        <v>19</v>
+      </c>
+      <c r="H12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="10" t="n">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="14" t="inlineStr">
         <is>
           <t>GRAND TOTAL (ALL LANGUAGES)</t>
         </is>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" s="10" t="inlineStr">
+    <row r="15">
+      <c r="A15" s="10" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B14" s="25" t="n">
-        <v>86.59999999999999</v>
-      </c>
-      <c r="C14" s="25" t="n">
+      <c r="B15" s="25" t="n">
+        <v>89.09999999999999</v>
+      </c>
+      <c r="C15" s="25" t="n">
         <v>100</v>
       </c>
-      <c r="D14" s="10" t="n">
-        <v>842</v>
-      </c>
-      <c r="E14" s="10" t="n">
-        <v>147</v>
-      </c>
-      <c r="F14" s="10" t="n">
-        <v>678</v>
-      </c>
-      <c r="G14" s="10" t="n">
-        <v>17</v>
-      </c>
-      <c r="H14" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K14" s="10" t="n">
-        <v>147</v>
+      <c r="D15" s="10" t="n">
+        <v>885</v>
+      </c>
+      <c r="E15" s="10" t="n">
+        <v>159</v>
+      </c>
+      <c r="F15" s="10" t="n">
+        <v>707</v>
+      </c>
+      <c r="G15" s="10" t="n">
+        <v>19</v>
+      </c>
+      <c r="H15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10" t="n">
+        <v>159</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
+    <mergeCell ref="A14:K14"/>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A13:K13"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
@@ -2534,7 +2690,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2841,19 +2997,19 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>379</v>
+        <v>391</v>
       </c>
       <c r="E7" t="n">
-        <v>342</v>
+        <v>347</v>
       </c>
       <c r="F7" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G7" t="n">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="H7" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -2885,16 +3041,16 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="E8" t="n">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="F8" t="n">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G8" t="n">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -2929,7 +3085,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
@@ -2973,16 +3129,16 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>257</v>
+        <v>262</v>
       </c>
       <c r="E10" t="n">
-        <v>229</v>
+        <v>249</v>
       </c>
       <c r="F10" t="n">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="G10" t="n">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -3017,16 +3173,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E11" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F11" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
@@ -3041,6 +3197,94 @@
         <v>0</v>
       </c>
       <c r="L11" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Quest</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>0</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2026-01-09</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Quest</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
QAExcelCompiler: Clear AutoFilter before sorting (clean slate)
- Added AutoFilter clearing in sort_worksheet_az() before sorting
- Added AutoFilter clearing in get_or_create_master() when creating from template
- Ensures clean slate before applying A-Z sort for Item category
- Testers may have filters applied - now properly cleared

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -2071,31 +2071,23 @@
           <t>--</t>
         </is>
       </c>
-      <c r="F8" s="21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="G8" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="H8" s="21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="I8" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+      <c r="F8" s="21" t="n">
+        <v>385</v>
+      </c>
+      <c r="G8" s="9" t="n">
+        <v>104</v>
+      </c>
+      <c r="H8" s="21" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" s="9" t="n">
+        <v>1</v>
       </c>
       <c r="J8" s="21" t="n">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="K8" s="9" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L8" s="21" t="n">
         <v>32</v>
@@ -2103,24 +2095,20 @@
       <c r="M8" s="9" t="n">
         <v>4</v>
       </c>
-      <c r="N8" s="21" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
-      </c>
-      <c r="O8" s="9" t="inlineStr">
-        <is>
-          <t>--</t>
-        </is>
+      <c r="N8" s="21" t="n">
+        <v>37</v>
+      </c>
+      <c r="O8" s="9" t="n">
+        <v>17</v>
       </c>
       <c r="P8" s="21" t="n">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="Q8" s="9" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="R8" s="21" t="n">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="S8" s="9" t="n">
         <v>63</v>
@@ -2146,7 +2134,7 @@
         </is>
       </c>
       <c r="X8" s="9" t="n">
-        <v>154</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -2341,22 +2329,22 @@
         </is>
       </c>
       <c r="B5" s="23" t="n">
-        <v>0</v>
+        <v>99.7</v>
       </c>
       <c r="C5" s="23" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="E5" s="8" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="F5" s="8" t="n">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="G5" s="8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H5" s="8" t="n">
         <v>0</v>
@@ -2368,7 +2356,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="8" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
@@ -2378,22 +2366,22 @@
         </is>
       </c>
       <c r="B6" s="24" t="n">
-        <v>0</v>
+        <v>37.5</v>
       </c>
       <c r="C6" s="24" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D6" s="9" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E6" s="9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="9" t="n">
         <v>0</v>
@@ -2405,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -2421,16 +2409,16 @@
         <v>100</v>
       </c>
       <c r="D7" s="8" t="n">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="E7" s="8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H7" s="8" t="n">
         <v>0</v>
@@ -2442,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -2489,19 +2477,19 @@
         </is>
       </c>
       <c r="B9" s="23" t="n">
-        <v>0</v>
+        <v>97.40000000000001</v>
       </c>
       <c r="C9" s="23" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="E9" s="8" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G9" s="8" t="n">
         <v>0</v>
@@ -2516,7 +2504,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="8" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -2526,19 +2514,19 @@
         </is>
       </c>
       <c r="B10" s="24" t="n">
-        <v>95</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="C10" s="24" t="n">
         <v>100</v>
       </c>
       <c r="D10" s="9" t="n">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="E10" s="9" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F10" s="9" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>0</v>
@@ -2553,7 +2541,7 @@
         <v>0</v>
       </c>
       <c r="K10" s="9" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="11">
@@ -2563,19 +2551,19 @@
         </is>
       </c>
       <c r="B11" s="23" t="n">
-        <v>95</v>
+        <v>96.90000000000001</v>
       </c>
       <c r="C11" s="23" t="n">
         <v>100</v>
       </c>
       <c r="D11" s="8" t="n">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="E11" s="8" t="n">
         <v>63</v>
       </c>
       <c r="F11" s="8" t="n">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="G11" s="8" t="n">
         <v>0</v>
@@ -2600,22 +2588,22 @@
         </is>
       </c>
       <c r="B12" s="25" t="n">
-        <v>89.09999999999999</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="C12" s="25" t="n">
         <v>100</v>
       </c>
       <c r="D12" s="10" t="n">
-        <v>885</v>
+        <v>1326</v>
       </c>
       <c r="E12" s="10" t="n">
-        <v>159</v>
+        <v>285</v>
       </c>
       <c r="F12" s="10" t="n">
-        <v>707</v>
+        <v>1012</v>
       </c>
       <c r="G12" s="10" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H12" s="10" t="n">
         <v>0</v>
@@ -2627,7 +2615,7 @@
         <v>0</v>
       </c>
       <c r="K12" s="10" t="n">
-        <v>159</v>
+        <v>285</v>
       </c>
     </row>
     <row r="14">
@@ -2644,22 +2632,22 @@
         </is>
       </c>
       <c r="B15" s="25" t="n">
-        <v>89.09999999999999</v>
+        <v>95.09999999999999</v>
       </c>
       <c r="C15" s="25" t="n">
         <v>100</v>
       </c>
       <c r="D15" s="10" t="n">
-        <v>885</v>
+        <v>1326</v>
       </c>
       <c r="E15" s="10" t="n">
-        <v>159</v>
+        <v>285</v>
       </c>
       <c r="F15" s="10" t="n">
-        <v>707</v>
+        <v>1012</v>
       </c>
       <c r="G15" s="10" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="H15" s="10" t="n">
         <v>0</v>
@@ -2671,7 +2659,7 @@
         <v>0</v>
       </c>
       <c r="K15" s="10" t="n">
-        <v>159</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2953,19 +2941,19 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>386</v>
       </c>
       <c r="E6" t="n">
-        <v>0</v>
+        <v>385</v>
       </c>
       <c r="F6" t="n">
-        <v>0</v>
+        <v>104</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>276</v>
       </c>
       <c r="H6" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
@@ -3044,13 +3032,13 @@
         <v>262</v>
       </c>
       <c r="E8" t="n">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="F8" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G8" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -3088,13 +3076,13 @@
         <v>38</v>
       </c>
       <c r="E9" t="n">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H9" t="n">
         <v>0</v>
@@ -3132,13 +3120,13 @@
         <v>262</v>
       </c>
       <c r="E10" t="n">
-        <v>249</v>
+        <v>254</v>
       </c>
       <c r="F10" t="n">
         <v>63</v>
       </c>
       <c r="G10" t="n">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="H10" t="n">
         <v>0</v>
@@ -3217,19 +3205,19 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E12" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
         <v>0</v>
@@ -3261,19 +3249,19 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E13" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I13" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
QAExcelCompiler: Ranking now uses SCALAR values (Done + Actual Issues)
Changed from percentage-based to scalar-based ranking:
- Score = 0.7 * Done + 0.3 * ActualIssues (scalar counts)
- Headers: Done, Actual Issues, Score
- Removed percentage formatting

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -18,8 +18,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0&quot;%&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -45,7 +46,7 @@
       <sz val="12"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="12">
     <fill>
       <patternFill/>
     </fill>
@@ -92,6 +93,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="005B2C6F"/>
+        <bgColor rgb="005B2C6F"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00C0C0C0"/>
+        <bgColor rgb="00C0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00CD7F32"/>
+        <bgColor rgb="00CD7F32"/>
       </patternFill>
     </fill>
   </fills>
@@ -168,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -235,6 +254,40 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="7" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -311,862 +364,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Daily Progress: Done by Tester</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Alice</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$B$5:$B$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Bob</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="ED7D31"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$D$5:$D$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>Doni</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="70AD47"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$F$5:$F$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <v>Eric</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="FFC000"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$H$5:$H$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <v>John</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="5B9BD5"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$J$5:$J$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <v>Jojo</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$L$5:$L$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <v>Lisa</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$N$5:$N$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="7"/>
-          <order val="7"/>
-          <tx>
-            <v>Mike</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$P$5:$P$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="8"/>
-          <order val="8"/>
-          <tx>
-            <v>Paul</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'DAILY'!$R$5:$R$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Date</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <tickLblPos val="low"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Done</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="b"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Progress: Done by Tester</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Alice</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Bob</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="ED7D31"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>Doni</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="70AD47"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$5</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <v>Eric</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="FFC000"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <v>John</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="5B9BD5"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <v>Jojo</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <v>Lisa</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$9</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="7"/>
-          <order val="7"/>
-          <tx>
-            <v>Mike</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$10</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="8"/>
-          <order val="8"/>
-          <tx>
-            <v>Paul</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$D$11</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <delete val="1"/>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Done</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="b"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="10"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Total Progress: Actual Issues % by Tester</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <barChart>
-        <barDir val="col"/>
-        <grouping val="clustered"/>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <v>Alice</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$3</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <v>Bob</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="ED7D31"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$4</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <v>Doni</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="70AD47"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$5</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="3"/>
-          <order val="3"/>
-          <tx>
-            <v>Eric</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="FFC000"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$6</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="4"/>
-          <order val="4"/>
-          <tx>
-            <v>John</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="5B9BD5"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$7</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="5"/>
-          <order val="5"/>
-          <tx>
-            <v>Jojo</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="7030A0"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$8</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="6"/>
-          <order val="6"/>
-          <tx>
-            <v>Lisa</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="C00000"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$9</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="7"/>
-          <order val="7"/>
-          <tx>
-            <v>Mike</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="00B0F0"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$10</f>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="8"/>
-          <order val="8"/>
-          <tx>
-            <v>Paul</v>
-          </tx>
-          <spPr>
-            <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:srgbClr val="4472C4"/>
-            </a:solidFill>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <val>
-            <numRef>
-              <f>'TOTAL'!$C$11</f>
-            </numRef>
-          </val>
-        </ser>
-        <gapWidth val="150"/>
-        <axId val="10"/>
-        <axId val="100"/>
-      </barChart>
-      <catAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <delete val="1"/>
-        <axPos val="l"/>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="100"/>
-        <lblOffset val="100"/>
-      </catAx>
-      <valAx>
-        <axId val="100"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Actual Issues %</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="b"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>9</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="3600000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>17</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8640000" cy="3600000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-  <oneCellAnchor>
-    <from>
-      <col>0</col>
-      <colOff>0</colOff>
-      <row>32</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="8640000" cy="3600000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="2" name="Chart 2"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2153,7 +1350,6 @@
     <mergeCell ref="H3:I3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2163,7 +1359,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:N43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2173,15 +1369,18 @@
   <cols>
     <col width="6" customWidth="1" min="1" max="1"/>
     <col width="12" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="7" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="9" customWidth="1" min="7" max="7"/>
-    <col width="7" customWidth="1" min="8" max="8"/>
+    <col width="8" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
     <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="10" customWidth="1" min="10" max="10"/>
-    <col width="9" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="10" max="10"/>
+    <col width="10" customWidth="1" min="11" max="11"/>
+    <col width="8" customWidth="1" min="12" max="12"/>
+    <col width="10" customWidth="1" min="13" max="13"/>
+    <col width="12" customWidth="1" min="14" max="14"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2662,13 +1861,984 @@
         <v>285</v>
       </c>
     </row>
+    <row r="18">
+      <c r="A18" s="12" t="inlineStr">
+        <is>
+          <t>EN CATEGORY BREAKDOWN (Words)</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="13" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="B19" s="13" t="inlineStr">
+        <is>
+          <t>Quest</t>
+        </is>
+      </c>
+      <c r="C19" s="26" t="n"/>
+      <c r="D19" s="13" t="inlineStr">
+        <is>
+          <t>Knowledge</t>
+        </is>
+      </c>
+      <c r="E19" s="26" t="n"/>
+      <c r="F19" s="13" t="inlineStr">
+        <is>
+          <t>Item</t>
+        </is>
+      </c>
+      <c r="G19" s="26" t="n"/>
+      <c r="H19" s="13" t="inlineStr">
+        <is>
+          <t>Region</t>
+        </is>
+      </c>
+      <c r="I19" s="26" t="n"/>
+      <c r="J19" s="13" t="inlineStr">
+        <is>
+          <t>System</t>
+        </is>
+      </c>
+      <c r="K19" s="26" t="n"/>
+      <c r="L19" s="13" t="inlineStr">
+        <is>
+          <t>Character</t>
+        </is>
+      </c>
+      <c r="M19" s="26" t="n"/>
+      <c r="N19" s="13" t="inlineStr">
+        <is>
+          <t>Total Words</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="26" t="inlineStr"/>
+      <c r="B20" s="27" t="inlineStr">
+        <is>
+          <t>Done%</t>
+        </is>
+      </c>
+      <c r="C20" s="27" t="inlineStr">
+        <is>
+          <t>Words</t>
+        </is>
+      </c>
+      <c r="D20" s="27" t="inlineStr">
+        <is>
+          <t>Done%</t>
+        </is>
+      </c>
+      <c r="E20" s="27" t="inlineStr">
+        <is>
+          <t>Words</t>
+        </is>
+      </c>
+      <c r="F20" s="27" t="inlineStr">
+        <is>
+          <t>Done%</t>
+        </is>
+      </c>
+      <c r="G20" s="27" t="inlineStr">
+        <is>
+          <t>Words</t>
+        </is>
+      </c>
+      <c r="H20" s="27" t="inlineStr">
+        <is>
+          <t>Done%</t>
+        </is>
+      </c>
+      <c r="I20" s="27" t="inlineStr">
+        <is>
+          <t>Words</t>
+        </is>
+      </c>
+      <c r="J20" s="27" t="inlineStr">
+        <is>
+          <t>Done%</t>
+        </is>
+      </c>
+      <c r="K20" s="27" t="inlineStr">
+        <is>
+          <t>Words</t>
+        </is>
+      </c>
+      <c r="L20" s="27" t="inlineStr">
+        <is>
+          <t>Done%</t>
+        </is>
+      </c>
+      <c r="M20" s="27" t="inlineStr">
+        <is>
+          <t>Words</t>
+        </is>
+      </c>
+      <c r="N20" s="26" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="8" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="B21" s="23" t="n">
+        <v>100</v>
+      </c>
+      <c r="C21" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M21" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N21" s="28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="9" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="B22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D22" s="24" t="n">
+        <v>100</v>
+      </c>
+      <c r="E22" s="29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M22" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N22" s="29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="inlineStr">
+        <is>
+          <t>Doni</t>
+        </is>
+      </c>
+      <c r="B23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D23" s="23" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="E23" s="28" t="n">
+        <v>5743</v>
+      </c>
+      <c r="F23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M23" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N23" s="28" t="n">
+        <v>5743</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="9" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="B24" s="24" t="n">
+        <v>37.5</v>
+      </c>
+      <c r="C24" s="29" t="n">
+        <v>11</v>
+      </c>
+      <c r="D24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M24" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N24" s="29" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="B25" s="23" t="n">
+        <v>87.5</v>
+      </c>
+      <c r="C25" s="28" t="n">
+        <v>21</v>
+      </c>
+      <c r="D25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F25" s="23" t="n">
+        <v>88.7</v>
+      </c>
+      <c r="G25" s="28" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M25" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N25" s="28" t="n">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="9" t="inlineStr">
+        <is>
+          <t>Jojo</t>
+        </is>
+      </c>
+      <c r="B26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="I26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="J26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K26" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L26" s="24" t="n">
+        <v>100</v>
+      </c>
+      <c r="M26" s="29" t="n">
+        <v>57</v>
+      </c>
+      <c r="N26" s="29" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="B27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H27" s="23" t="n">
+        <v>97.40000000000001</v>
+      </c>
+      <c r="I27" s="28" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M27" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N27" s="28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="9" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="B28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" s="24" t="n">
+        <v>96.59999999999999</v>
+      </c>
+      <c r="I28" s="29" t="n">
+        <v>1979</v>
+      </c>
+      <c r="J28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M28" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N28" s="29" t="n">
+        <v>1979</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="B29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H29" s="23" t="n">
+        <v>96.90000000000001</v>
+      </c>
+      <c r="I29" s="28" t="n">
+        <v>1962</v>
+      </c>
+      <c r="J29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M29" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N29" s="28" t="n">
+        <v>1962</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="10" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="B30" s="25" t="n">
+        <v>71.40000000000001</v>
+      </c>
+      <c r="C30" s="30" t="n">
+        <v>32</v>
+      </c>
+      <c r="D30" s="25" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="E30" s="30" t="n">
+        <v>5743</v>
+      </c>
+      <c r="F30" s="25" t="n">
+        <v>88.7</v>
+      </c>
+      <c r="G30" s="30" t="n">
+        <v>1025</v>
+      </c>
+      <c r="H30" s="25" t="n">
+        <v>96.8</v>
+      </c>
+      <c r="I30" s="30" t="n">
+        <v>3941</v>
+      </c>
+      <c r="J30" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="K30" s="10" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L30" s="25" t="n">
+        <v>100</v>
+      </c>
+      <c r="M30" s="30" t="n">
+        <v>57</v>
+      </c>
+      <c r="N30" s="30" t="n">
+        <v>10798</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="12" t="inlineStr">
+        <is>
+          <t>EN RANKING (70% Done + 30% Actual Issues)</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="13" t="inlineStr">
+        <is>
+          <t>Rank</t>
+        </is>
+      </c>
+      <c r="B34" s="13" t="inlineStr">
+        <is>
+          <t>User</t>
+        </is>
+      </c>
+      <c r="C34" s="13" t="inlineStr">
+        <is>
+          <t>Done</t>
+        </is>
+      </c>
+      <c r="D34" s="13" t="inlineStr">
+        <is>
+          <t>Actual Issues</t>
+        </is>
+      </c>
+      <c r="E34" s="13" t="inlineStr">
+        <is>
+          <t>Score</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="B35" s="33" t="inlineStr">
+        <is>
+          <t>Doni</t>
+        </is>
+      </c>
+      <c r="C35" s="8" t="n">
+        <v>385</v>
+      </c>
+      <c r="D35" s="8" t="n">
+        <v>104</v>
+      </c>
+      <c r="E35" s="34" t="n">
+        <v>300.7</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="35" t="n">
+        <v>2</v>
+      </c>
+      <c r="B36" s="33" t="inlineStr">
+        <is>
+          <t>John</t>
+        </is>
+      </c>
+      <c r="C36" s="8" t="n">
+        <v>354</v>
+      </c>
+      <c r="D36" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="E36" s="34" t="n">
+        <v>249.9</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="36" t="n">
+        <v>3</v>
+      </c>
+      <c r="B37" s="33" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="C37" s="8" t="n">
+        <v>253</v>
+      </c>
+      <c r="D37" s="8" t="n">
+        <v>86</v>
+      </c>
+      <c r="E37" s="34" t="n">
+        <v>202.9</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B38" s="9" t="inlineStr">
+        <is>
+          <t>Paul</t>
+        </is>
+      </c>
+      <c r="C38" s="9" t="n">
+        <v>254</v>
+      </c>
+      <c r="D38" s="9" t="n">
+        <v>63</v>
+      </c>
+      <c r="E38" s="37" t="n">
+        <v>196.7</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B39" s="8" t="inlineStr">
+        <is>
+          <t>Lisa</t>
+        </is>
+      </c>
+      <c r="C39" s="8" t="n">
+        <v>37</v>
+      </c>
+      <c r="D39" s="8" t="n">
+        <v>17</v>
+      </c>
+      <c r="E39" s="34" t="n">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B40" s="9" t="inlineStr">
+        <is>
+          <t>Jojo</t>
+        </is>
+      </c>
+      <c r="C40" s="9" t="n">
+        <v>32</v>
+      </c>
+      <c r="D40" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" s="37" t="n">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B41" s="8" t="inlineStr">
+        <is>
+          <t>Alice</t>
+        </is>
+      </c>
+      <c r="C41" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D41" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E41" s="34" t="n">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="9" t="n">
+        <v>8</v>
+      </c>
+      <c r="B42" s="9" t="inlineStr">
+        <is>
+          <t>Bob</t>
+        </is>
+      </c>
+      <c r="C42" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="D42" s="9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E42" s="37" t="n">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="8" t="n">
+        <v>9</v>
+      </c>
+      <c r="B43" s="8" t="inlineStr">
+        <is>
+          <t>Eric</t>
+        </is>
+      </c>
+      <c r="C43" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D43" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="E43" s="34" t="n">
+        <v>2.4</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
+    <mergeCell ref="A18:N18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="L19:M19"/>
     <mergeCell ref="A14:K14"/>
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2678,7 +2848,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2747,6 +2917,11 @@
           <t>NonIssue</t>
         </is>
       </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>WordCount</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -2967,6 +3142,9 @@
       <c r="L6" t="n">
         <v>0</v>
       </c>
+      <c r="M6" t="n">
+        <v>5743</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -3011,6 +3189,9 @@
       <c r="L7" t="n">
         <v>0</v>
       </c>
+      <c r="M7" t="n">
+        <v>1025</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -3055,6 +3236,9 @@
       <c r="L8" t="n">
         <v>0</v>
       </c>
+      <c r="M8" t="n">
+        <v>1979</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -3099,6 +3283,9 @@
       <c r="L9" t="n">
         <v>0</v>
       </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -3143,6 +3330,9 @@
       <c r="L10" t="n">
         <v>0</v>
       </c>
+      <c r="M10" t="n">
+        <v>1962</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -3187,6 +3377,9 @@
       <c r="L11" t="n">
         <v>0</v>
       </c>
+      <c r="M11" t="n">
+        <v>57</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -3231,6 +3424,9 @@
       <c r="L12" t="n">
         <v>0</v>
       </c>
+      <c r="M12" t="n">
+        <v>11</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -3274,6 +3470,9 @@
       </c>
       <c r="L13" t="n">
         <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QAExcelCompiler: Simplify TOTAL stats table - remove Completion%, rename Total to Done
- Removed "Completion" and "Actual Issues" columns from TOTAL stats (already in Category Breakdown)
- Renamed "Total" → "Done" for consistency with DAILY sheet
- Headers now: User, Done, Issues, No Issue, Blocked, Fixed, Reported, Checking, Pending
- Cleaner, less confusing when adding new categories

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
+++ b/RessourcesForCodingTheProject/NewScripts/QAExcelCompiler/LQA_Tester_ProgressTracker.xlsx
@@ -1398,50 +1398,40 @@
       </c>
       <c r="B2" s="13" t="inlineStr">
         <is>
-          <t>Completion</t>
+          <t>Done</t>
         </is>
       </c>
       <c r="C2" s="13" t="inlineStr">
         <is>
-          <t>Actual Issues</t>
+          <t>Issues</t>
         </is>
       </c>
       <c r="D2" s="13" t="inlineStr">
         <is>
-          <t>Total</t>
+          <t>No Issue</t>
         </is>
       </c>
       <c r="E2" s="13" t="inlineStr">
         <is>
-          <t>Issues</t>
-        </is>
-      </c>
-      <c r="F2" s="13" t="inlineStr">
-        <is>
-          <t>No Issue</t>
-        </is>
-      </c>
-      <c r="G2" s="13" t="inlineStr">
-        <is>
           <t>Blocked</t>
         </is>
       </c>
+      <c r="F2" s="5" t="inlineStr">
+        <is>
+          <t>Fixed</t>
+        </is>
+      </c>
+      <c r="G2" s="5" t="inlineStr">
+        <is>
+          <t>Reported</t>
+        </is>
+      </c>
       <c r="H2" s="5" t="inlineStr">
         <is>
-          <t>Fixed</t>
+          <t>Checking</t>
         </is>
       </c>
       <c r="I2" s="5" t="inlineStr">
-        <is>
-          <t>Reported</t>
-        </is>
-      </c>
-      <c r="J2" s="5" t="inlineStr">
-        <is>
-          <t>Checking</t>
-        </is>
-      </c>
-      <c r="K2" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1453,20 +1443,20 @@
           <t>Alice</t>
         </is>
       </c>
-      <c r="B3" s="23" t="n">
-        <v>100</v>
-      </c>
-      <c r="C3" s="23" t="n">
-        <v>100</v>
+      <c r="B3" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <v>1</v>
       </c>
       <c r="D3" s="8" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" s="8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" s="8" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="G3" s="8" t="n">
         <v>0</v>
@@ -1475,12 +1465,6 @@
         <v>0</v>
       </c>
       <c r="I3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="8" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1490,20 +1474,20 @@
           <t>Bob</t>
         </is>
       </c>
-      <c r="B4" s="24" t="n">
-        <v>100</v>
-      </c>
-      <c r="C4" s="24" t="n">
-        <v>100</v>
+      <c r="B4" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>2</v>
       </c>
       <c r="D4" s="9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="9" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F4" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G4" s="9" t="n">
         <v>0</v>
@@ -1512,12 +1496,6 @@
         <v>0</v>
       </c>
       <c r="I4" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1527,34 +1505,28 @@
           <t>Doni</t>
         </is>
       </c>
-      <c r="B5" s="23" t="n">
-        <v>99.7</v>
-      </c>
-      <c r="C5" s="23" t="n">
-        <v>100</v>
+      <c r="B5" s="8" t="n">
+        <v>385</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <v>104</v>
       </c>
       <c r="D5" s="8" t="n">
-        <v>385</v>
+        <v>276</v>
       </c>
       <c r="E5" s="8" t="n">
-        <v>104</v>
+        <v>5</v>
       </c>
       <c r="F5" s="8" t="n">
-        <v>276</v>
+        <v>0</v>
       </c>
       <c r="G5" s="8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H5" s="8" t="n">
         <v>0</v>
       </c>
       <c r="I5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8" t="n">
         <v>104</v>
       </c>
     </row>
@@ -1564,34 +1536,28 @@
           <t>Eric</t>
         </is>
       </c>
-      <c r="B6" s="24" t="n">
-        <v>37.5</v>
-      </c>
-      <c r="C6" s="24" t="n">
-        <v>100</v>
+      <c r="B6" s="9" t="n">
+        <v>3</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>1</v>
       </c>
       <c r="D6" s="9" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="F6" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="9" t="n">
         <v>0</v>
       </c>
       <c r="I6" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1601,34 +1567,28 @@
           <t>John</t>
         </is>
       </c>
-      <c r="B7" s="23" t="n">
-        <v>88.7</v>
-      </c>
-      <c r="C7" s="23" t="n">
-        <v>100</v>
+      <c r="B7" s="8" t="n">
+        <v>354</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <v>7</v>
       </c>
       <c r="D7" s="8" t="n">
-        <v>354</v>
+        <v>324</v>
       </c>
       <c r="E7" s="8" t="n">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="F7" s="8" t="n">
-        <v>324</v>
+        <v>0</v>
       </c>
       <c r="G7" s="8" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="H7" s="8" t="n">
         <v>0</v>
       </c>
       <c r="I7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1638,20 +1598,20 @@
           <t>Jojo</t>
         </is>
       </c>
-      <c r="B8" s="24" t="n">
-        <v>100</v>
-      </c>
-      <c r="C8" s="24" t="n">
-        <v>100</v>
+      <c r="B8" s="9" t="n">
+        <v>32</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>4</v>
       </c>
       <c r="D8" s="9" t="n">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E8" s="9" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F8" s="9" t="n">
-        <v>28</v>
+        <v>0</v>
       </c>
       <c r="G8" s="9" t="n">
         <v>0</v>
@@ -1660,12 +1620,6 @@
         <v>0</v>
       </c>
       <c r="I8" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9" t="n">
         <v>4</v>
       </c>
     </row>
@@ -1675,20 +1629,20 @@
           <t>Lisa</t>
         </is>
       </c>
-      <c r="B9" s="23" t="n">
-        <v>97.40000000000001</v>
-      </c>
-      <c r="C9" s="23" t="n">
-        <v>100</v>
+      <c r="B9" s="8" t="n">
+        <v>37</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <v>17</v>
       </c>
       <c r="D9" s="8" t="n">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E9" s="8" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="F9" s="8" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="G9" s="8" t="n">
         <v>0</v>
@@ -1697,12 +1651,6 @@
         <v>0</v>
       </c>
       <c r="I9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="8" t="n">
         <v>17</v>
       </c>
     </row>
@@ -1712,20 +1660,20 @@
           <t>Mike</t>
         </is>
       </c>
-      <c r="B10" s="24" t="n">
-        <v>96.59999999999999</v>
-      </c>
-      <c r="C10" s="24" t="n">
-        <v>100</v>
+      <c r="B10" s="9" t="n">
+        <v>253</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>86</v>
       </c>
       <c r="D10" s="9" t="n">
-        <v>253</v>
+        <v>167</v>
       </c>
       <c r="E10" s="9" t="n">
-        <v>86</v>
+        <v>0</v>
       </c>
       <c r="F10" s="9" t="n">
-        <v>167</v>
+        <v>0</v>
       </c>
       <c r="G10" s="9" t="n">
         <v>0</v>
@@ -1734,12 +1682,6 @@
         <v>0</v>
       </c>
       <c r="I10" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9" t="n">
         <v>86</v>
       </c>
     </row>
@@ -1749,20 +1691,20 @@
           <t>Paul</t>
         </is>
       </c>
-      <c r="B11" s="23" t="n">
-        <v>96.90000000000001</v>
-      </c>
-      <c r="C11" s="23" t="n">
-        <v>100</v>
+      <c r="B11" s="8" t="n">
+        <v>254</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <v>63</v>
       </c>
       <c r="D11" s="8" t="n">
-        <v>254</v>
+        <v>191</v>
       </c>
       <c r="E11" s="8" t="n">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="F11" s="8" t="n">
-        <v>191</v>
+        <v>0</v>
       </c>
       <c r="G11" s="8" t="n">
         <v>0</v>
@@ -1771,12 +1713,6 @@
         <v>0</v>
       </c>
       <c r="I11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8" t="n">
         <v>63</v>
       </c>
     </row>
@@ -1786,34 +1722,28 @@
           <t>SUBTOTAL</t>
         </is>
       </c>
-      <c r="B12" s="25" t="n">
-        <v>95.09999999999999</v>
-      </c>
-      <c r="C12" s="25" t="n">
-        <v>100</v>
+      <c r="B12" s="10" t="n">
+        <v>1326</v>
+      </c>
+      <c r="C12" s="10" t="n">
+        <v>285</v>
       </c>
       <c r="D12" s="10" t="n">
-        <v>1326</v>
+        <v>1012</v>
       </c>
       <c r="E12" s="10" t="n">
-        <v>285</v>
+        <v>29</v>
       </c>
       <c r="F12" s="10" t="n">
-        <v>1012</v>
+        <v>0</v>
       </c>
       <c r="G12" s="10" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H12" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="10" t="n">
         <v>285</v>
       </c>
     </row>
@@ -1830,34 +1760,28 @@
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="B15" s="25" t="n">
-        <v>95.09999999999999</v>
-      </c>
-      <c r="C15" s="25" t="n">
-        <v>100</v>
+      <c r="B15" s="10" t="n">
+        <v>1326</v>
+      </c>
+      <c r="C15" s="10" t="n">
+        <v>285</v>
       </c>
       <c r="D15" s="10" t="n">
-        <v>1326</v>
+        <v>1012</v>
       </c>
       <c r="E15" s="10" t="n">
-        <v>285</v>
+        <v>29</v>
       </c>
       <c r="F15" s="10" t="n">
-        <v>1012</v>
+        <v>0</v>
       </c>
       <c r="G15" s="10" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="H15" s="10" t="n">
         <v>0</v>
       </c>
       <c r="I15" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="10" t="n">
         <v>285</v>
       </c>
     </row>
@@ -2830,13 +2754,13 @@
     <mergeCell ref="A18:N18"/>
     <mergeCell ref="D19:E19"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="A14:I14"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="A33:E33"/>
+    <mergeCell ref="A1:I1"/>
     <mergeCell ref="J19:K19"/>
     <mergeCell ref="H19:I19"/>
     <mergeCell ref="L19:M19"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>